<commit_message>
Model cores of cpu instead of jobslots
Ignore jobslots for the beginning, implement them later as passive
resources for each resource container.
</commit_message>
<xml_diff>
--- a/data/summary_gridka_data.xlsx
+++ b/data/summary_gridka_data.xlsx
@@ -512,7 +512,7 @@
   <dimension ref="A1:U1294"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="U25" sqref="U25"/>
+      <selection activeCell="P26" sqref="P26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,6 +1872,10 @@
       <c r="L26">
         <f>((L2*S2+L3*S3+L4*S4+L5*S5+L6*S6+L7*S7+L8*S8+L9*S9+L10*S10+L11*S11+L12*S12+L13*S13+L14*S14+L15*S15+L16*S16+L17*S17+L18*S18+L19*S19+L20*S20+L21*S21)/S23)</f>
         <v>334.94563031709203</v>
+      </c>
+      <c r="P26">
+        <f>((P2*S2+P3*S3+P4*S4+P5*S5+P6*S6+P7*S7+P8*S8+P9*S9+P10*S10+P11*S11+P12*S12+P13*S13+P14*S14+P15*S15+P16*S16+P17*S17+P18*S18+P19*S19+P20*S20+P21*S21)/S23)</f>
+        <v>18.895591647331788</v>
       </c>
       <c r="R26">
         <f>((R2*S2+R3*S3+R4*S4+R5*S5+R6*S6+R7*S7+R8*S8+R9*S9+R10*S10+R11*S11+R12*S12+R13*S13+R14*S14+R15*S15+R16*S16+R17*S17+R18*S18+R19*S19+R20*S20+R21*S21)/S23)</f>

</xml_diff>